<commit_message>
code source cleanup and implementation of the generated in the spreadsheet into the H2 databse
</commit_message>
<xml_diff>
--- a/intel.xlsx
+++ b/intel.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="72">
   <si>
     <t>Intel</t>
   </si>
@@ -58,10 +58,10 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>Código do produto:</t>
-  </si>
-  <si>
-    <t>WEWE893AAE</t>
+    <t>Product code:</t>
+  </si>
+  <si>
+    <t>OI9SKG581H</t>
   </si>
   <si>
     <t>Date:</t>
@@ -88,9 +88,6 @@
     <t>2018-01-12T02:00:00Z</t>
   </si>
   <si>
-    <t>NULL</t>
-  </si>
-  <si>
     <t>HARDWARE</t>
   </si>
   <si>
@@ -145,7 +142,7 @@
     <t>480.00 R$</t>
   </si>
   <si>
-    <t>5O4RT45X88</t>
+    <t>GEEWOAY1LH</t>
   </si>
   <si>
     <t>12/02/2018</t>
@@ -154,7 +151,7 @@
     <t>2018-02-12T02:00:00Z</t>
   </si>
   <si>
-    <t>OWGDZ0ZIF3</t>
+    <t>SYSGPVQI2N</t>
   </si>
   <si>
     <t>12/03/2018</t>
@@ -163,7 +160,7 @@
     <t>2018-03-12T03:00:00Z</t>
   </si>
   <si>
-    <t>3O3YX074UB</t>
+    <t>KT8AVO8XA8</t>
   </si>
   <si>
     <t>12/04/2018</t>
@@ -172,7 +169,7 @@
     <t>2018-04-12T03:00:00Z</t>
   </si>
   <si>
-    <t>BV98N7RG7A</t>
+    <t>305TZION5W</t>
   </si>
   <si>
     <t>12/05/2018</t>
@@ -181,7 +178,7 @@
     <t>2018-05-12T03:00:00Z</t>
   </si>
   <si>
-    <t>WXKUBHRXX8</t>
+    <t>EX2KPI4S8H</t>
   </si>
   <si>
     <t>12/06/2018</t>
@@ -190,7 +187,7 @@
     <t>2018-06-12T03:00:00Z</t>
   </si>
   <si>
-    <t>U650HCARIB</t>
+    <t>AVG3FMMNED</t>
   </si>
   <si>
     <t>12/07/2018</t>
@@ -199,7 +196,7 @@
     <t>2018-07-12T03:00:00Z</t>
   </si>
   <si>
-    <t>CII14RU3LZ</t>
+    <t>CXR9F31RI7</t>
   </si>
   <si>
     <t>12/08/2018</t>
@@ -208,7 +205,7 @@
     <t>2018-08-12T03:00:00Z</t>
   </si>
   <si>
-    <t>KGJBPNXTQ6</t>
+    <t>GRN1J1G1IW</t>
   </si>
   <si>
     <t>12/09/2018</t>
@@ -217,7 +214,7 @@
     <t>2018-09-12T03:00:00Z</t>
   </si>
   <si>
-    <t>3FGE5Z9H2Q</t>
+    <t>CVCBTPX4Y9</t>
   </si>
   <si>
     <t>12/10/2018</t>
@@ -226,7 +223,7 @@
     <t>2018-10-12T03:00:00Z</t>
   </si>
   <si>
-    <t>QMNRP2UP83</t>
+    <t>1IE3CVPXFU</t>
   </si>
   <si>
     <t>12/11/2018</t>
@@ -235,7 +232,7 @@
     <t>2018-11-12T02:00:00Z</t>
   </si>
   <si>
-    <t>N5VEVOBFWA</t>
+    <t>K2WYT6NLBF</t>
   </si>
   <si>
     <t>12/12/2018</t>
@@ -1752,7 +1749,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="21.76953125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="17.02734375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="14.16796875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="19.84765625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="11.08984375" customWidth="true" bestFit="true"/>
@@ -1760,7 +1757,7 @@
     <col min="6" max="6" width="21.2734375" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="14.6796875" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="11.7265625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="14.06640625" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="12.91796875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="30.0" customHeight="true">
@@ -1835,139 +1832,124 @@
       <c r="F6" t="s">
         <v>20</v>
       </c>
-      <c r="G6" t="s">
-        <v>21</v>
-      </c>
       <c r="H6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I6" t="s">
         <v>12</v>
       </c>
       <c r="J6" t="n">
-        <v>8.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>24</v>
-      </c>
-      <c r="E7" t="s">
-        <v>25</v>
       </c>
       <c r="F7" t="s">
         <v>20</v>
       </c>
-      <c r="G7" t="s">
-        <v>21</v>
-      </c>
       <c r="H7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I7" t="s">
         <v>12</v>
       </c>
       <c r="J7" t="n">
-        <v>16.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
         <v>26</v>
       </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>27</v>
-      </c>
-      <c r="E8" t="s">
-        <v>28</v>
       </c>
       <c r="F8" t="s">
         <v>20</v>
       </c>
-      <c r="G8" t="s">
-        <v>21</v>
-      </c>
       <c r="H8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I8" t="s">
         <v>12</v>
       </c>
       <c r="J8" t="n">
-        <v>15.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
         <v>29</v>
       </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>30</v>
-      </c>
-      <c r="E9" t="s">
-        <v>31</v>
       </c>
       <c r="F9" t="s">
         <v>20</v>
       </c>
-      <c r="G9" t="s">
-        <v>21</v>
-      </c>
       <c r="H9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I9" t="s">
         <v>12</v>
       </c>
       <c r="J9" t="n">
-        <v>11.0</v>
+        <v>17.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
         <v>32</v>
       </c>
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>33</v>
-      </c>
-      <c r="E10" t="s">
-        <v>34</v>
       </c>
       <c r="F10" t="s">
         <v>20</v>
       </c>
-      <c r="G10" t="s">
-        <v>21</v>
-      </c>
       <c r="H10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I10" t="s">
         <v>12</v>
@@ -1978,7 +1960,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
         <v>16</v>
@@ -1990,16 +1972,13 @@
         <v>19</v>
       </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F11" t="s">
         <v>20</v>
       </c>
-      <c r="G11" t="s">
-        <v>21</v>
-      </c>
       <c r="H11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I11" t="s">
         <v>12</v>
@@ -2010,34 +1989,31 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
         <v>37</v>
       </c>
-      <c r="B12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>38</v>
-      </c>
-      <c r="E12" t="s">
-        <v>39</v>
       </c>
       <c r="F12" t="s">
         <v>20</v>
       </c>
-      <c r="G12" t="s">
-        <v>21</v>
-      </c>
       <c r="H12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I12" t="s">
         <v>12</v>
       </c>
       <c r="J12" t="n">
-        <v>12.0</v>
+        <v>3.0</v>
       </c>
     </row>
   </sheetData>
@@ -2058,7 +2034,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="21.76953125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="17.02734375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="14.16796875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="19.84765625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="11.08984375" customWidth="true" bestFit="true"/>
@@ -2079,7 +2055,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s" s="148">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4">
@@ -2087,7 +2063,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s" s="150">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5">
@@ -2139,80 +2115,71 @@
         <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>66</v>
-      </c>
-      <c r="G6" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="H6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J6" t="n">
-        <v>5.0</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>24</v>
       </c>
-      <c r="E7" t="s">
-        <v>25</v>
-      </c>
       <c r="F7" t="s">
-        <v>66</v>
-      </c>
-      <c r="G7" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="H7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J7" t="n">
-        <v>11.0</v>
+        <v>19.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
         <v>26</v>
       </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>27</v>
       </c>
-      <c r="E8" t="s">
-        <v>28</v>
-      </c>
       <c r="F8" t="s">
-        <v>66</v>
-      </c>
-      <c r="G8" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="H8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J8" t="n">
         <v>9.0</v>
@@ -2220,71 +2187,65 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
         <v>29</v>
       </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>30</v>
       </c>
-      <c r="E9" t="s">
-        <v>31</v>
-      </c>
       <c r="F9" t="s">
-        <v>66</v>
-      </c>
-      <c r="G9" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="H9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J9" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
         <v>32</v>
       </c>
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>33</v>
       </c>
-      <c r="E10" t="s">
-        <v>34</v>
-      </c>
       <c r="F10" t="s">
-        <v>66</v>
-      </c>
-      <c r="G10" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="H10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J10" t="n">
-        <v>5.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
         <v>16</v>
@@ -2296,54 +2257,48 @@
         <v>19</v>
       </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F11" t="s">
-        <v>66</v>
-      </c>
-      <c r="G11" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="H11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J11" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
         <v>37</v>
       </c>
-      <c r="B12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>38</v>
       </c>
-      <c r="E12" t="s">
-        <v>39</v>
-      </c>
       <c r="F12" t="s">
-        <v>66</v>
-      </c>
-      <c r="G12" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="H12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J12" t="n">
-        <v>17.0</v>
+        <v>15.0</v>
       </c>
     </row>
   </sheetData>
@@ -2364,7 +2319,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="21.76953125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="17.02734375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="14.16796875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="19.84765625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="11.08984375" customWidth="true" bestFit="true"/>
@@ -2372,7 +2327,7 @@
     <col min="6" max="6" width="21.2734375" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="14.6796875" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="11.7265625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="14.04296875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="12.91796875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="30.0" customHeight="true">
@@ -2385,7 +2340,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s" s="163">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4">
@@ -2393,7 +2348,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s" s="165">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5">
@@ -2445,80 +2400,71 @@
         <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>69</v>
-      </c>
-      <c r="G6" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="H6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J6" t="n">
-        <v>13.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>24</v>
       </c>
-      <c r="E7" t="s">
-        <v>25</v>
-      </c>
       <c r="F7" t="s">
-        <v>69</v>
-      </c>
-      <c r="G7" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="H7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J7" t="n">
-        <v>13.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
         <v>26</v>
       </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>27</v>
       </c>
-      <c r="E8" t="s">
-        <v>28</v>
-      </c>
       <c r="F8" t="s">
-        <v>69</v>
-      </c>
-      <c r="G8" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="H8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J8" t="n">
         <v>10.0</v>
@@ -2526,71 +2472,65 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
         <v>29</v>
       </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>30</v>
       </c>
-      <c r="E9" t="s">
-        <v>31</v>
-      </c>
       <c r="F9" t="s">
-        <v>69</v>
-      </c>
-      <c r="G9" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="H9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J9" t="n">
-        <v>13.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
         <v>32</v>
       </c>
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>33</v>
       </c>
-      <c r="E10" t="s">
-        <v>34</v>
-      </c>
       <c r="F10" t="s">
-        <v>69</v>
-      </c>
-      <c r="G10" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="H10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J10" t="n">
-        <v>12.0</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
         <v>16</v>
@@ -2602,54 +2542,48 @@
         <v>19</v>
       </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F11" t="s">
-        <v>69</v>
-      </c>
-      <c r="G11" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="H11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J11" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
         <v>37</v>
       </c>
-      <c r="B12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>38</v>
       </c>
-      <c r="E12" t="s">
-        <v>39</v>
-      </c>
       <c r="F12" t="s">
-        <v>69</v>
-      </c>
-      <c r="G12" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="H12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J12" t="n">
-        <v>11.0</v>
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>
@@ -2670,7 +2604,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="21.76953125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="17.02734375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="14.16796875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="19.84765625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="11.08984375" customWidth="true" bestFit="true"/>
@@ -2678,7 +2612,7 @@
     <col min="6" max="6" width="21.2734375" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="14.6796875" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="11.7265625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="14.0390625" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="13.06640625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="30.0" customHeight="true">
@@ -2691,7 +2625,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s" s="178">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4">
@@ -2699,7 +2633,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s" s="180">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5">
@@ -2751,48 +2685,42 @@
         <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>72</v>
-      </c>
-      <c r="G6" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="H6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J6" t="n">
-        <v>13.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>24</v>
       </c>
-      <c r="E7" t="s">
-        <v>25</v>
-      </c>
       <c r="F7" t="s">
-        <v>72</v>
-      </c>
-      <c r="G7" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="H7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J7" t="n">
         <v>12.0</v>
@@ -2800,103 +2728,94 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
         <v>26</v>
       </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>27</v>
       </c>
-      <c r="E8" t="s">
-        <v>28</v>
-      </c>
       <c r="F8" t="s">
-        <v>72</v>
-      </c>
-      <c r="G8" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="H8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J8" t="n">
-        <v>9.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
         <v>29</v>
       </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>30</v>
       </c>
-      <c r="E9" t="s">
-        <v>31</v>
-      </c>
       <c r="F9" t="s">
-        <v>72</v>
-      </c>
-      <c r="G9" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="H9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J9" t="n">
-        <v>7.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
         <v>32</v>
       </c>
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>33</v>
       </c>
-      <c r="E10" t="s">
-        <v>34</v>
-      </c>
       <c r="F10" t="s">
-        <v>72</v>
-      </c>
-      <c r="G10" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="H10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J10" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
         <v>16</v>
@@ -2908,54 +2827,48 @@
         <v>19</v>
       </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F11" t="s">
-        <v>72</v>
-      </c>
-      <c r="G11" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="H11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J11" t="n">
-        <v>18.0</v>
+        <v>14.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
         <v>37</v>
       </c>
-      <c r="B12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>38</v>
       </c>
-      <c r="E12" t="s">
-        <v>39</v>
-      </c>
       <c r="F12" t="s">
-        <v>72</v>
-      </c>
-      <c r="G12" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="H12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J12" t="n">
-        <v>6.0</v>
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>
@@ -2976,7 +2889,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="21.76953125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="17.02734375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="14.16796875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="19.84765625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="11.08984375" customWidth="true" bestFit="true"/>
@@ -2984,7 +2897,7 @@
     <col min="6" max="6" width="21.2734375" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="14.6796875" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="11.7265625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="12.91796875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="13.7421875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="30.0" customHeight="true">
@@ -2997,7 +2910,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s" s="28">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4">
@@ -3005,7 +2918,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s" s="30">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5">
@@ -3057,152 +2970,137 @@
         <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>42</v>
-      </c>
-      <c r="G6" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="H6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J6" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>24</v>
       </c>
-      <c r="E7" t="s">
-        <v>25</v>
-      </c>
       <c r="F7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G7" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="H7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J7" t="n">
-        <v>6.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
         <v>26</v>
       </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>27</v>
       </c>
-      <c r="E8" t="s">
-        <v>28</v>
-      </c>
       <c r="F8" t="s">
-        <v>42</v>
-      </c>
-      <c r="G8" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="H8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J8" t="n">
-        <v>8.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
         <v>29</v>
       </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>30</v>
       </c>
-      <c r="E9" t="s">
-        <v>31</v>
-      </c>
       <c r="F9" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="H9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J9" t="n">
-        <v>15.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
         <v>32</v>
       </c>
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>33</v>
       </c>
-      <c r="E10" t="s">
-        <v>34</v>
-      </c>
       <c r="F10" t="s">
-        <v>42</v>
-      </c>
-      <c r="G10" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="H10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J10" t="n">
-        <v>15.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
         <v>16</v>
@@ -3214,19 +3112,16 @@
         <v>19</v>
       </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F11" t="s">
-        <v>42</v>
-      </c>
-      <c r="G11" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="H11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J11" t="n">
         <v>14.0</v>
@@ -3234,34 +3129,31 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
         <v>37</v>
       </c>
-      <c r="B12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>38</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" t="s">
         <v>39</v>
       </c>
-      <c r="F12" t="s">
-        <v>42</v>
-      </c>
-      <c r="G12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H12" t="s">
-        <v>22</v>
-      </c>
-      <c r="I12" t="s">
-        <v>40</v>
-      </c>
       <c r="J12" t="n">
-        <v>19.0</v>
+        <v>6.0</v>
       </c>
     </row>
   </sheetData>
@@ -3282,7 +3174,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="21.76953125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="17.02734375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="14.16796875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="19.84765625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="11.08984375" customWidth="true" bestFit="true"/>
@@ -3290,7 +3182,7 @@
     <col min="6" max="6" width="21.2734375" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="14.6796875" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="11.7265625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="13.046875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="12.91796875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="30.0" customHeight="true">
@@ -3303,7 +3195,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s" s="43">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4">
@@ -3311,7 +3203,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s" s="45">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5">
@@ -3363,112 +3255,100 @@
         <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>45</v>
-      </c>
-      <c r="G6" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="H6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J6" t="n">
-        <v>6.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>24</v>
       </c>
-      <c r="E7" t="s">
-        <v>25</v>
-      </c>
       <c r="F7" t="s">
-        <v>45</v>
-      </c>
-      <c r="G7" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="H7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J7" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
         <v>26</v>
       </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>27</v>
       </c>
-      <c r="E8" t="s">
-        <v>28</v>
-      </c>
       <c r="F8" t="s">
-        <v>45</v>
-      </c>
-      <c r="G8" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="H8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J8" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
         <v>29</v>
       </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>30</v>
       </c>
-      <c r="E9" t="s">
-        <v>31</v>
-      </c>
       <c r="F9" t="s">
-        <v>45</v>
-      </c>
-      <c r="G9" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="H9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J9" t="n">
         <v>14.0</v>
@@ -3476,39 +3356,36 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
         <v>32</v>
       </c>
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>33</v>
       </c>
-      <c r="E10" t="s">
-        <v>34</v>
-      </c>
       <c r="F10" t="s">
-        <v>45</v>
-      </c>
-      <c r="G10" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="H10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J10" t="n">
-        <v>17.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
         <v>16</v>
@@ -3520,54 +3397,48 @@
         <v>19</v>
       </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F11" t="s">
-        <v>45</v>
-      </c>
-      <c r="G11" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="H11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J11" t="n">
-        <v>9.0</v>
+        <v>19.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
         <v>37</v>
       </c>
-      <c r="B12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>38</v>
       </c>
-      <c r="E12" t="s">
-        <v>39</v>
-      </c>
       <c r="F12" t="s">
-        <v>45</v>
-      </c>
-      <c r="G12" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="H12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J12" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>
@@ -3588,7 +3459,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="21.76953125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="17.02734375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="14.16796875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="19.84765625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="11.08984375" customWidth="true" bestFit="true"/>
@@ -3596,7 +3467,7 @@
     <col min="6" max="6" width="21.2734375" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="14.6796875" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="11.7265625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="12.91796875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="12.9921875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="30.0" customHeight="true">
@@ -3609,7 +3480,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s" s="58">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4">
@@ -3617,7 +3488,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s" s="60">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5">
@@ -3669,152 +3540,137 @@
         <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>48</v>
-      </c>
-      <c r="G6" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="H6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J6" t="n">
-        <v>6.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>24</v>
       </c>
-      <c r="E7" t="s">
-        <v>25</v>
-      </c>
       <c r="F7" t="s">
-        <v>48</v>
-      </c>
-      <c r="G7" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="H7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J7" t="n">
-        <v>13.0</v>
+        <v>18.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
         <v>26</v>
       </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>27</v>
       </c>
-      <c r="E8" t="s">
-        <v>28</v>
-      </c>
       <c r="F8" t="s">
-        <v>48</v>
-      </c>
-      <c r="G8" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="H8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J8" t="n">
-        <v>9.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
         <v>29</v>
       </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>30</v>
       </c>
-      <c r="E9" t="s">
-        <v>31</v>
-      </c>
       <c r="F9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G9" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="H9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J9" t="n">
-        <v>10.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
         <v>32</v>
       </c>
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>33</v>
       </c>
-      <c r="E10" t="s">
-        <v>34</v>
-      </c>
       <c r="F10" t="s">
-        <v>48</v>
-      </c>
-      <c r="G10" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="H10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J10" t="n">
-        <v>17.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
         <v>16</v>
@@ -3826,54 +3682,48 @@
         <v>19</v>
       </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F11" t="s">
-        <v>48</v>
-      </c>
-      <c r="G11" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="H11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J11" t="n">
-        <v>5.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
         <v>37</v>
       </c>
-      <c r="B12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>38</v>
       </c>
-      <c r="E12" t="s">
-        <v>39</v>
-      </c>
       <c r="F12" t="s">
-        <v>48</v>
-      </c>
-      <c r="G12" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="H12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J12" t="n">
-        <v>4.0</v>
+        <v>18.0</v>
       </c>
     </row>
   </sheetData>
@@ -3894,7 +3744,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="21.76953125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="17.02734375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="14.16796875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="19.84765625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="11.08984375" customWidth="true" bestFit="true"/>
@@ -3902,7 +3752,7 @@
     <col min="6" max="6" width="21.2734375" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="14.6796875" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="11.7265625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="13.21875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="12.98828125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="30.0" customHeight="true">
@@ -3915,7 +3765,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s" s="73">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4">
@@ -3923,7 +3773,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s" s="75">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5">
@@ -3975,152 +3825,137 @@
         <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>51</v>
-      </c>
-      <c r="G6" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="H6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J6" t="n">
-        <v>14.0</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>24</v>
       </c>
-      <c r="E7" t="s">
-        <v>25</v>
-      </c>
       <c r="F7" t="s">
-        <v>51</v>
-      </c>
-      <c r="G7" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="H7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J7" t="n">
-        <v>13.0</v>
+        <v>17.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
         <v>26</v>
       </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>27</v>
       </c>
-      <c r="E8" t="s">
-        <v>28</v>
-      </c>
       <c r="F8" t="s">
-        <v>51</v>
-      </c>
-      <c r="G8" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="H8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J8" t="n">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
         <v>29</v>
       </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>30</v>
       </c>
-      <c r="E9" t="s">
-        <v>31</v>
-      </c>
       <c r="F9" t="s">
-        <v>51</v>
-      </c>
-      <c r="G9" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="H9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J9" t="n">
-        <v>7.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
         <v>32</v>
       </c>
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>33</v>
       </c>
-      <c r="E10" t="s">
-        <v>34</v>
-      </c>
       <c r="F10" t="s">
-        <v>51</v>
-      </c>
-      <c r="G10" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="H10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J10" t="n">
-        <v>7.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
         <v>16</v>
@@ -4132,54 +3967,48 @@
         <v>19</v>
       </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F11" t="s">
-        <v>51</v>
-      </c>
-      <c r="G11" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="H11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J11" t="n">
-        <v>4.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
         <v>37</v>
       </c>
-      <c r="B12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>38</v>
       </c>
-      <c r="E12" t="s">
-        <v>39</v>
-      </c>
       <c r="F12" t="s">
-        <v>51</v>
-      </c>
-      <c r="G12" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="H12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J12" t="n">
-        <v>18.0</v>
+        <v>14.0</v>
       </c>
     </row>
   </sheetData>
@@ -4200,7 +4029,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="21.76953125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="17.02734375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="14.16796875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="19.84765625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="11.08984375" customWidth="true" bestFit="true"/>
@@ -4208,7 +4037,7 @@
     <col min="6" max="6" width="21.2734375" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="14.6796875" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="11.7265625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="13.8515625" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="12.91796875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="30.0" customHeight="true">
@@ -4221,7 +4050,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s" s="88">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4">
@@ -4229,7 +4058,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s" s="90">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5">
@@ -4281,112 +4110,100 @@
         <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>54</v>
-      </c>
-      <c r="G6" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="H6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J6" t="n">
-        <v>15.0</v>
+        <v>19.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>24</v>
       </c>
-      <c r="E7" t="s">
-        <v>25</v>
-      </c>
       <c r="F7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G7" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="H7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J7" t="n">
-        <v>7.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
         <v>26</v>
       </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>27</v>
       </c>
-      <c r="E8" t="s">
-        <v>28</v>
-      </c>
       <c r="F8" t="s">
-        <v>54</v>
-      </c>
-      <c r="G8" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="H8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J8" t="n">
-        <v>12.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
         <v>29</v>
       </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>30</v>
       </c>
-      <c r="E9" t="s">
-        <v>31</v>
-      </c>
       <c r="F9" t="s">
-        <v>54</v>
-      </c>
-      <c r="G9" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="H9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J9" t="n">
         <v>16.0</v>
@@ -4394,39 +4211,36 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
         <v>32</v>
       </c>
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>33</v>
       </c>
-      <c r="E10" t="s">
-        <v>34</v>
-      </c>
       <c r="F10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G10" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="H10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J10" t="n">
-        <v>10.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
         <v>16</v>
@@ -4438,54 +4252,48 @@
         <v>19</v>
       </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F11" t="s">
-        <v>54</v>
-      </c>
-      <c r="G11" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="H11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J11" t="n">
-        <v>7.0</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
         <v>37</v>
       </c>
-      <c r="B12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>38</v>
       </c>
-      <c r="E12" t="s">
-        <v>39</v>
-      </c>
       <c r="F12" t="s">
-        <v>54</v>
-      </c>
-      <c r="G12" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="H12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J12" t="n">
-        <v>3.0</v>
+        <v>17.0</v>
       </c>
     </row>
   </sheetData>
@@ -4506,7 +4314,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="21.76953125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="17.02734375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="14.16796875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="19.84765625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="11.08984375" customWidth="true" bestFit="true"/>
@@ -4514,7 +4322,7 @@
     <col min="6" max="6" width="21.2734375" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="14.6796875" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="11.7265625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="12.91796875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="14.68359375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="30.0" customHeight="true">
@@ -4527,7 +4335,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s" s="103">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4">
@@ -4535,7 +4343,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s" s="105">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5">
@@ -4587,152 +4395,137 @@
         <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G6" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="H6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J6" t="n">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>24</v>
       </c>
-      <c r="E7" t="s">
-        <v>25</v>
-      </c>
       <c r="F7" t="s">
-        <v>57</v>
-      </c>
-      <c r="G7" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="H7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J7" t="n">
-        <v>7.0</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
         <v>26</v>
       </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>27</v>
       </c>
-      <c r="E8" t="s">
-        <v>28</v>
-      </c>
       <c r="F8" t="s">
-        <v>57</v>
-      </c>
-      <c r="G8" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="H8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J8" t="n">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
         <v>29</v>
       </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>30</v>
       </c>
-      <c r="E9" t="s">
-        <v>31</v>
-      </c>
       <c r="F9" t="s">
-        <v>57</v>
-      </c>
-      <c r="G9" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="H9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J9" t="n">
-        <v>6.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
         <v>32</v>
       </c>
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>33</v>
       </c>
-      <c r="E10" t="s">
-        <v>34</v>
-      </c>
       <c r="F10" t="s">
-        <v>57</v>
-      </c>
-      <c r="G10" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="H10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J10" t="n">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
         <v>16</v>
@@ -4744,54 +4537,48 @@
         <v>19</v>
       </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F11" t="s">
-        <v>57</v>
-      </c>
-      <c r="G11" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="H11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J11" t="n">
-        <v>6.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
         <v>37</v>
       </c>
-      <c r="B12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>38</v>
       </c>
-      <c r="E12" t="s">
-        <v>39</v>
-      </c>
       <c r="F12" t="s">
-        <v>57</v>
-      </c>
-      <c r="G12" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="H12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J12" t="n">
-        <v>7.0</v>
+        <v>15.0</v>
       </c>
     </row>
   </sheetData>
@@ -4812,7 +4599,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="21.76953125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="17.02734375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="14.16796875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="19.84765625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="11.08984375" customWidth="true" bestFit="true"/>
@@ -4833,7 +4620,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s" s="118">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4">
@@ -4841,7 +4628,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s" s="120">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5">
@@ -4893,152 +4680,137 @@
         <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>60</v>
-      </c>
-      <c r="G6" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="H6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J6" t="n">
-        <v>14.0</v>
+        <v>18.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>24</v>
       </c>
-      <c r="E7" t="s">
-        <v>25</v>
-      </c>
       <c r="F7" t="s">
-        <v>60</v>
-      </c>
-      <c r="G7" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="H7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J7" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
         <v>26</v>
       </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>27</v>
       </c>
-      <c r="E8" t="s">
-        <v>28</v>
-      </c>
       <c r="F8" t="s">
-        <v>60</v>
-      </c>
-      <c r="G8" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="H8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J8" t="n">
-        <v>13.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
         <v>29</v>
       </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>30</v>
       </c>
-      <c r="E9" t="s">
-        <v>31</v>
-      </c>
       <c r="F9" t="s">
-        <v>60</v>
-      </c>
-      <c r="G9" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="H9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J9" t="n">
-        <v>0.0</v>
+        <v>16.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
         <v>32</v>
       </c>
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>33</v>
       </c>
-      <c r="E10" t="s">
-        <v>34</v>
-      </c>
       <c r="F10" t="s">
-        <v>60</v>
-      </c>
-      <c r="G10" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="H10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J10" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
         <v>16</v>
@@ -5050,54 +4822,48 @@
         <v>19</v>
       </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F11" t="s">
-        <v>60</v>
-      </c>
-      <c r="G11" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="H11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J11" t="n">
-        <v>13.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
         <v>37</v>
       </c>
-      <c r="B12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>38</v>
       </c>
-      <c r="E12" t="s">
-        <v>39</v>
-      </c>
       <c r="F12" t="s">
-        <v>60</v>
-      </c>
-      <c r="G12" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="H12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J12" t="n">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
     </row>
   </sheetData>
@@ -5118,7 +4884,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="21.76953125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="17.02734375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="14.16796875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="19.84765625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="11.08984375" customWidth="true" bestFit="true"/>
@@ -5126,7 +4892,7 @@
     <col min="6" max="6" width="21.2734375" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="14.6796875" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="11.7265625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="12.91796875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="12.984375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="30.0" customHeight="true">
@@ -5139,7 +4905,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s" s="133">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4">
@@ -5147,7 +4913,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s" s="135">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5">
@@ -5199,152 +4965,137 @@
         <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>63</v>
-      </c>
-      <c r="G6" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="H6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J6" t="n">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>24</v>
       </c>
-      <c r="E7" t="s">
-        <v>25</v>
-      </c>
       <c r="F7" t="s">
-        <v>63</v>
-      </c>
-      <c r="G7" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="H7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J7" t="n">
-        <v>17.0</v>
+        <v>18.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
         <v>26</v>
       </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>27</v>
       </c>
-      <c r="E8" t="s">
-        <v>28</v>
-      </c>
       <c r="F8" t="s">
-        <v>63</v>
-      </c>
-      <c r="G8" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="H8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J8" t="n">
-        <v>15.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
         <v>29</v>
       </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>30</v>
       </c>
-      <c r="E9" t="s">
-        <v>31</v>
-      </c>
       <c r="F9" t="s">
-        <v>63</v>
-      </c>
-      <c r="G9" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="H9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J9" t="n">
-        <v>17.0</v>
+        <v>11.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
         <v>32</v>
       </c>
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>33</v>
       </c>
-      <c r="E10" t="s">
-        <v>34</v>
-      </c>
       <c r="F10" t="s">
-        <v>63</v>
-      </c>
-      <c r="G10" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="H10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J10" t="n">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
         <v>16</v>
@@ -5356,54 +5107,48 @@
         <v>19</v>
       </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F11" t="s">
-        <v>63</v>
-      </c>
-      <c r="G11" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="H11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J11" t="n">
-        <v>13.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
         <v>37</v>
       </c>
-      <c r="B12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>38</v>
       </c>
-      <c r="E12" t="s">
-        <v>39</v>
-      </c>
       <c r="F12" t="s">
-        <v>63</v>
-      </c>
-      <c r="G12" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="H12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J12" t="n">
-        <v>7.0</v>
+        <v>9.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Using the program to generate data
</commit_message>
<xml_diff>
--- a/intel.xlsx
+++ b/intel.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="133">
   <si>
     <t>Intel</t>
   </si>
@@ -61,13 +61,13 @@
     <t>Product code:</t>
   </si>
   <si>
-    <t>OI9SKG581H</t>
+    <t>LAI15K6G1Y</t>
   </si>
   <si>
     <t>Date:</t>
   </si>
   <si>
-    <t>12/01/2018</t>
+    <t>12/01/2015</t>
   </si>
   <si>
     <t>Intel Core i3-8100</t>
@@ -79,60 +79,72 @@
     <t>http://wgfgfdgd.com</t>
   </si>
   <si>
-    <t>200.000 R$</t>
+    <t>200.00 R$</t>
+  </si>
+  <si>
+    <t>300.0 R$</t>
+  </si>
+  <si>
+    <t>04/02/2015</t>
+  </si>
+  <si>
+    <t>HARDWARE</t>
+  </si>
+  <si>
+    <t>Intel Core i5-6400</t>
+  </si>
+  <si>
+    <t>400.00 R$</t>
+  </si>
+  <si>
+    <t>600.0 R$</t>
+  </si>
+  <si>
+    <t>17/01/2015</t>
+  </si>
+  <si>
+    <t>Intel Core i5-8500</t>
+  </si>
+  <si>
+    <t>600.00 R$</t>
+  </si>
+  <si>
+    <t>700.0 R$</t>
+  </si>
+  <si>
+    <t>26/01/2015</t>
+  </si>
+  <si>
+    <t>Intel Core i5-8400</t>
+  </si>
+  <si>
+    <t>550.00 R$</t>
+  </si>
+  <si>
+    <t>650.0 R$</t>
+  </si>
+  <si>
+    <t>07/02/2015</t>
+  </si>
+  <si>
+    <t>Intel Core i5-500</t>
+  </si>
+  <si>
+    <t>100.00 R$</t>
+  </si>
+  <si>
+    <t>500.00 R$</t>
+  </si>
+  <si>
+    <t>03/02/2015</t>
+  </si>
+  <si>
+    <t>Intel Core i7-500</t>
   </si>
   <si>
     <t>300.00 R$</t>
   </si>
   <si>
-    <t>2018-01-12T02:00:00Z</t>
-  </si>
-  <si>
-    <t>HARDWARE</t>
-  </si>
-  <si>
-    <t>Intel Core i5-6400</t>
-  </si>
-  <si>
-    <t>400.000 R$</t>
-  </si>
-  <si>
-    <t>600.00 R$</t>
-  </si>
-  <si>
-    <t>Intel Core i5-8500</t>
-  </si>
-  <si>
-    <t>600.000 R$</t>
-  </si>
-  <si>
-    <t>700.00 R$</t>
-  </si>
-  <si>
-    <t>Intel Core i5-8400</t>
-  </si>
-  <si>
-    <t>550.00 R$</t>
-  </si>
-  <si>
-    <t>650.00 R$</t>
-  </si>
-  <si>
-    <t>Intel Core i5-500</t>
-  </si>
-  <si>
-    <t>100.00 R$</t>
-  </si>
-  <si>
-    <t>500.00 R$</t>
-  </si>
-  <si>
-    <t>Intel Core i7-500</t>
-  </si>
-  <si>
-    <t>400.00 R$</t>
-  </si>
-  <si>
     <t>Intel Core i3-6400</t>
   </si>
   <si>
@@ -142,103 +154,274 @@
     <t>480.00 R$</t>
   </si>
   <si>
-    <t>GEEWOAY1LH</t>
-  </si>
-  <si>
-    <t>12/02/2018</t>
-  </si>
-  <si>
-    <t>2018-02-12T02:00:00Z</t>
-  </si>
-  <si>
-    <t>SYSGPVQI2N</t>
-  </si>
-  <si>
-    <t>12/03/2018</t>
-  </si>
-  <si>
-    <t>2018-03-12T03:00:00Z</t>
-  </si>
-  <si>
-    <t>KT8AVO8XA8</t>
-  </si>
-  <si>
-    <t>12/04/2018</t>
-  </si>
-  <si>
-    <t>2018-04-12T03:00:00Z</t>
-  </si>
-  <si>
-    <t>305TZION5W</t>
-  </si>
-  <si>
-    <t>12/05/2018</t>
-  </si>
-  <si>
-    <t>2018-05-12T03:00:00Z</t>
-  </si>
-  <si>
-    <t>EX2KPI4S8H</t>
-  </si>
-  <si>
-    <t>12/06/2018</t>
-  </si>
-  <si>
-    <t>2018-06-12T03:00:00Z</t>
-  </si>
-  <si>
-    <t>AVG3FMMNED</t>
-  </si>
-  <si>
-    <t>12/07/2018</t>
-  </si>
-  <si>
-    <t>2018-07-12T03:00:00Z</t>
-  </si>
-  <si>
-    <t>CXR9F31RI7</t>
-  </si>
-  <si>
-    <t>12/08/2018</t>
-  </si>
-  <si>
-    <t>2018-08-12T03:00:00Z</t>
-  </si>
-  <si>
-    <t>GRN1J1G1IW</t>
-  </si>
-  <si>
-    <t>12/09/2018</t>
-  </si>
-  <si>
-    <t>2018-09-12T03:00:00Z</t>
-  </si>
-  <si>
-    <t>CVCBTPX4Y9</t>
-  </si>
-  <si>
-    <t>12/10/2018</t>
-  </si>
-  <si>
-    <t>2018-10-12T03:00:00Z</t>
-  </si>
-  <si>
-    <t>1IE3CVPXFU</t>
-  </si>
-  <si>
-    <t>12/11/2018</t>
-  </si>
-  <si>
-    <t>2018-11-12T02:00:00Z</t>
-  </si>
-  <si>
-    <t>K2WYT6NLBF</t>
-  </si>
-  <si>
-    <t>12/12/2018</t>
-  </si>
-  <si>
-    <t>2018-12-12T02:00:00Z</t>
+    <t>10/02/2015</t>
+  </si>
+  <si>
+    <t>T8T4GQD5U7</t>
+  </si>
+  <si>
+    <t>12/02/2015</t>
+  </si>
+  <si>
+    <t>02/03/2015</t>
+  </si>
+  <si>
+    <t>22/02/2015</t>
+  </si>
+  <si>
+    <t>12/03/2015</t>
+  </si>
+  <si>
+    <t>09/03/2015</t>
+  </si>
+  <si>
+    <t>01/03/2015</t>
+  </si>
+  <si>
+    <t>AQ6OK9TW61</t>
+  </si>
+  <si>
+    <t>28/03/2015</t>
+  </si>
+  <si>
+    <t>08/04/2015</t>
+  </si>
+  <si>
+    <t>05/04/2015</t>
+  </si>
+  <si>
+    <t>19/03/2015</t>
+  </si>
+  <si>
+    <t>01/04/2015</t>
+  </si>
+  <si>
+    <t>15/03/2015</t>
+  </si>
+  <si>
+    <t>27/03/2015</t>
+  </si>
+  <si>
+    <t>FKAEM4AHAI</t>
+  </si>
+  <si>
+    <t>12/04/2015</t>
+  </si>
+  <si>
+    <t>14/04/2015</t>
+  </si>
+  <si>
+    <t>24/04/2015</t>
+  </si>
+  <si>
+    <t>27/04/2015</t>
+  </si>
+  <si>
+    <t>20/04/2015</t>
+  </si>
+  <si>
+    <t>11/05/2015</t>
+  </si>
+  <si>
+    <t>05/05/2015</t>
+  </si>
+  <si>
+    <t>07/05/2015</t>
+  </si>
+  <si>
+    <t>CWH3ITFQNH</t>
+  </si>
+  <si>
+    <t>12/05/2015</t>
+  </si>
+  <si>
+    <t>21/05/2015</t>
+  </si>
+  <si>
+    <t>19/05/2015</t>
+  </si>
+  <si>
+    <t>28/05/2015</t>
+  </si>
+  <si>
+    <t>24/05/2015</t>
+  </si>
+  <si>
+    <t>08/06/2015</t>
+  </si>
+  <si>
+    <t>29/05/2015</t>
+  </si>
+  <si>
+    <t>05/06/2015</t>
+  </si>
+  <si>
+    <t>7X6ZKX74FM</t>
+  </si>
+  <si>
+    <t>12/06/2015</t>
+  </si>
+  <si>
+    <t>15/06/2015</t>
+  </si>
+  <si>
+    <t>10/07/2015</t>
+  </si>
+  <si>
+    <t>18/06/2015</t>
+  </si>
+  <si>
+    <t>16/06/2015</t>
+  </si>
+  <si>
+    <t>07/07/2015</t>
+  </si>
+  <si>
+    <t>26/06/2015</t>
+  </si>
+  <si>
+    <t>27/06/2015</t>
+  </si>
+  <si>
+    <t>EEPS2K0169</t>
+  </si>
+  <si>
+    <t>12/07/2015</t>
+  </si>
+  <si>
+    <t>10/08/2015</t>
+  </si>
+  <si>
+    <t>04/08/2015</t>
+  </si>
+  <si>
+    <t>14/07/2015</t>
+  </si>
+  <si>
+    <t>06/08/2015</t>
+  </si>
+  <si>
+    <t>01/08/2015</t>
+  </si>
+  <si>
+    <t>20/07/2015</t>
+  </si>
+  <si>
+    <t>911AILEN2I</t>
+  </si>
+  <si>
+    <t>12/08/2015</t>
+  </si>
+  <si>
+    <t>04/09/2015</t>
+  </si>
+  <si>
+    <t>01/09/2015</t>
+  </si>
+  <si>
+    <t>18/08/2015</t>
+  </si>
+  <si>
+    <t>26/08/2015</t>
+  </si>
+  <si>
+    <t>03/09/2015</t>
+  </si>
+  <si>
+    <t>28/08/2015</t>
+  </si>
+  <si>
+    <t>20/08/2015</t>
+  </si>
+  <si>
+    <t>OAHCGMS8H9</t>
+  </si>
+  <si>
+    <t>12/09/2015</t>
+  </si>
+  <si>
+    <t>19/09/2015</t>
+  </si>
+  <si>
+    <t>02/10/2015</t>
+  </si>
+  <si>
+    <t>04/10/2015</t>
+  </si>
+  <si>
+    <t>16/09/2015</t>
+  </si>
+  <si>
+    <t>23/09/2015</t>
+  </si>
+  <si>
+    <t>E0EDHH1AX1</t>
+  </si>
+  <si>
+    <t>12/10/2015</t>
+  </si>
+  <si>
+    <t>05/11/2015</t>
+  </si>
+  <si>
+    <t>23/10/2015</t>
+  </si>
+  <si>
+    <t>04/11/2015</t>
+  </si>
+  <si>
+    <t>29/10/2015</t>
+  </si>
+  <si>
+    <t>19/10/2015</t>
+  </si>
+  <si>
+    <t>IOQ32Y1G69</t>
+  </si>
+  <si>
+    <t>12/11/2015</t>
+  </si>
+  <si>
+    <t>11/12/2015</t>
+  </si>
+  <si>
+    <t>24/11/2015</t>
+  </si>
+  <si>
+    <t>29/11/2015</t>
+  </si>
+  <si>
+    <t>01/12/2015</t>
+  </si>
+  <si>
+    <t>23/11/2015</t>
+  </si>
+  <si>
+    <t>07/12/2015</t>
+  </si>
+  <si>
+    <t>5SM3CONEDI</t>
+  </si>
+  <si>
+    <t>12/12/2015</t>
+  </si>
+  <si>
+    <t>28/12/2015</t>
+  </si>
+  <si>
+    <t>30/12/2015</t>
+  </si>
+  <si>
+    <t>26/12/2015</t>
+  </si>
+  <si>
+    <t>21/12/2015</t>
+  </si>
+  <si>
+    <t>25/12/2015</t>
+  </si>
+  <si>
+    <t>14/12/2015</t>
   </si>
 </sst>
 </file>
@@ -1752,9 +1935,9 @@
     <col min="1" max="1" width="17.02734375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="14.16796875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="19.84765625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="11.08984375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="9.9765625" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="9.9765625" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="21.2734375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="13.28515625" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="14.6796875" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="11.7265625" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="12.91796875" customWidth="true" bestFit="true"/>
@@ -1830,6 +2013,9 @@
         <v>19</v>
       </c>
       <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" t="s">
         <v>20</v>
       </c>
       <c r="H6" t="s">
@@ -1839,7 +2025,7 @@
         <v>12</v>
       </c>
       <c r="J6" t="n">
-        <v>10.0</v>
+        <v>19.0</v>
       </c>
     </row>
     <row r="7">
@@ -1859,7 +2045,10 @@
         <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>14</v>
+      </c>
+      <c r="G7" t="s">
+        <v>25</v>
       </c>
       <c r="H7" t="s">
         <v>21</v>
@@ -1868,12 +2057,12 @@
         <v>12</v>
       </c>
       <c r="J7" t="n">
-        <v>4.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
@@ -1882,13 +2071,16 @@
         <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F8" t="s">
-        <v>20</v>
+        <v>14</v>
+      </c>
+      <c r="G8" t="s">
+        <v>29</v>
       </c>
       <c r="H8" t="s">
         <v>21</v>
@@ -1897,12 +2089,12 @@
         <v>12</v>
       </c>
       <c r="J8" t="n">
-        <v>6.0</v>
+        <v>18.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
         <v>16</v>
@@ -1911,13 +2103,16 @@
         <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F9" t="s">
-        <v>20</v>
+        <v>14</v>
+      </c>
+      <c r="G9" t="s">
+        <v>33</v>
       </c>
       <c r="H9" t="s">
         <v>21</v>
@@ -1926,12 +2121,12 @@
         <v>12</v>
       </c>
       <c r="J9" t="n">
-        <v>17.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
         <v>16</v>
@@ -1940,13 +2135,16 @@
         <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F10" t="s">
-        <v>20</v>
+        <v>14</v>
+      </c>
+      <c r="G10" t="s">
+        <v>37</v>
       </c>
       <c r="H10" t="s">
         <v>21</v>
@@ -1955,12 +2153,12 @@
         <v>12</v>
       </c>
       <c r="J10" t="n">
-        <v>4.0</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
         <v>16</v>
@@ -1969,13 +2167,16 @@
         <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="F11" t="s">
-        <v>20</v>
+        <v>14</v>
+      </c>
+      <c r="G11" t="s">
+        <v>14</v>
       </c>
       <c r="H11" t="s">
         <v>21</v>
@@ -1984,12 +2185,12 @@
         <v>12</v>
       </c>
       <c r="J11" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B12" t="s">
         <v>16</v>
@@ -1998,13 +2199,16 @@
         <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F12" t="s">
-        <v>20</v>
+        <v>14</v>
+      </c>
+      <c r="G12" t="s">
+        <v>43</v>
       </c>
       <c r="H12" t="s">
         <v>21</v>
@@ -2013,7 +2217,7 @@
         <v>12</v>
       </c>
       <c r="J12" t="n">
-        <v>3.0</v>
+        <v>9.0</v>
       </c>
     </row>
   </sheetData>
@@ -2037,12 +2241,12 @@
     <col min="1" max="1" width="17.02734375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="14.16796875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="19.84765625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="11.08984375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="9.9765625" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="9.9765625" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="21.2734375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="13.28515625" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="14.6796875" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="11.7265625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="12.91796875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="13.0390625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="30.0" customHeight="true">
@@ -2055,7 +2259,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s" s="148">
-        <v>63</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4">
@@ -2063,7 +2267,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s" s="150">
-        <v>64</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5">
@@ -2115,16 +2319,19 @@
         <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>65</v>
+        <v>111</v>
+      </c>
+      <c r="G6" t="s">
+        <v>112</v>
       </c>
       <c r="H6" t="s">
         <v>21</v>
       </c>
       <c r="I6" t="s">
-        <v>63</v>
+        <v>110</v>
       </c>
       <c r="J6" t="n">
-        <v>15.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="7">
@@ -2144,21 +2351,24 @@
         <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>65</v>
+        <v>111</v>
+      </c>
+      <c r="G7" t="s">
+        <v>112</v>
       </c>
       <c r="H7" t="s">
         <v>21</v>
       </c>
       <c r="I7" t="s">
-        <v>63</v>
+        <v>110</v>
       </c>
       <c r="J7" t="n">
-        <v>19.0</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
@@ -2167,27 +2377,30 @@
         <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F8" t="s">
-        <v>65</v>
+        <v>111</v>
+      </c>
+      <c r="G8" t="s">
+        <v>113</v>
       </c>
       <c r="H8" t="s">
         <v>21</v>
       </c>
       <c r="I8" t="s">
-        <v>63</v>
+        <v>110</v>
       </c>
       <c r="J8" t="n">
-        <v>9.0</v>
+        <v>16.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
         <v>16</v>
@@ -2196,27 +2409,30 @@
         <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F9" t="s">
-        <v>65</v>
+        <v>111</v>
+      </c>
+      <c r="G9" t="s">
+        <v>114</v>
       </c>
       <c r="H9" t="s">
         <v>21</v>
       </c>
       <c r="I9" t="s">
-        <v>63</v>
+        <v>110</v>
       </c>
       <c r="J9" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
         <v>16</v>
@@ -2225,27 +2441,30 @@
         <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F10" t="s">
-        <v>65</v>
+        <v>111</v>
+      </c>
+      <c r="G10" t="s">
+        <v>114</v>
       </c>
       <c r="H10" t="s">
         <v>21</v>
       </c>
       <c r="I10" t="s">
-        <v>63</v>
+        <v>110</v>
       </c>
       <c r="J10" t="n">
-        <v>12.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
         <v>16</v>
@@ -2254,27 +2473,30 @@
         <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="F11" t="s">
-        <v>65</v>
+        <v>111</v>
+      </c>
+      <c r="G11" t="s">
+        <v>115</v>
       </c>
       <c r="H11" t="s">
         <v>21</v>
       </c>
       <c r="I11" t="s">
-        <v>63</v>
+        <v>110</v>
       </c>
       <c r="J11" t="n">
-        <v>5.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B12" t="s">
         <v>16</v>
@@ -2283,22 +2505,25 @@
         <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F12" t="s">
-        <v>65</v>
+        <v>111</v>
+      </c>
+      <c r="G12" t="s">
+        <v>116</v>
       </c>
       <c r="H12" t="s">
         <v>21</v>
       </c>
       <c r="I12" t="s">
-        <v>63</v>
+        <v>110</v>
       </c>
       <c r="J12" t="n">
-        <v>15.0</v>
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>
@@ -2322,9 +2547,9 @@
     <col min="1" max="1" width="17.02734375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="14.16796875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="19.84765625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="11.08984375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="9.9765625" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="9.9765625" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="21.2734375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="13.28515625" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="14.6796875" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="11.7265625" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="12.91796875" customWidth="true" bestFit="true"/>
@@ -2340,7 +2565,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s" s="163">
-        <v>66</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4">
@@ -2348,7 +2573,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s" s="165">
-        <v>67</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5">
@@ -2400,16 +2625,19 @@
         <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>68</v>
+        <v>118</v>
+      </c>
+      <c r="G6" t="s">
+        <v>119</v>
       </c>
       <c r="H6" t="s">
         <v>21</v>
       </c>
       <c r="I6" t="s">
-        <v>66</v>
+        <v>117</v>
       </c>
       <c r="J6" t="n">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="7">
@@ -2429,21 +2657,24 @@
         <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>68</v>
+        <v>118</v>
+      </c>
+      <c r="G7" t="s">
+        <v>120</v>
       </c>
       <c r="H7" t="s">
         <v>21</v>
       </c>
       <c r="I7" t="s">
-        <v>66</v>
+        <v>117</v>
       </c>
       <c r="J7" t="n">
-        <v>8.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
@@ -2452,27 +2683,30 @@
         <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F8" t="s">
-        <v>68</v>
+        <v>118</v>
+      </c>
+      <c r="G8" t="s">
+        <v>121</v>
       </c>
       <c r="H8" t="s">
         <v>21</v>
       </c>
       <c r="I8" t="s">
-        <v>66</v>
+        <v>117</v>
       </c>
       <c r="J8" t="n">
-        <v>10.0</v>
+        <v>17.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
         <v>16</v>
@@ -2481,27 +2715,30 @@
         <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F9" t="s">
-        <v>68</v>
+        <v>118</v>
+      </c>
+      <c r="G9" t="s">
+        <v>122</v>
       </c>
       <c r="H9" t="s">
         <v>21</v>
       </c>
       <c r="I9" t="s">
-        <v>66</v>
+        <v>117</v>
       </c>
       <c r="J9" t="n">
-        <v>0.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
         <v>16</v>
@@ -2510,27 +2747,30 @@
         <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F10" t="s">
-        <v>68</v>
+        <v>118</v>
+      </c>
+      <c r="G10" t="s">
+        <v>123</v>
       </c>
       <c r="H10" t="s">
         <v>21</v>
       </c>
       <c r="I10" t="s">
-        <v>66</v>
+        <v>117</v>
       </c>
       <c r="J10" t="n">
-        <v>15.0</v>
+        <v>11.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
         <v>16</v>
@@ -2539,19 +2779,22 @@
         <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="F11" t="s">
-        <v>68</v>
+        <v>118</v>
+      </c>
+      <c r="G11" t="s">
+        <v>124</v>
       </c>
       <c r="H11" t="s">
         <v>21</v>
       </c>
       <c r="I11" t="s">
-        <v>66</v>
+        <v>117</v>
       </c>
       <c r="J11" t="n">
         <v>1.0</v>
@@ -2559,7 +2802,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B12" t="s">
         <v>16</v>
@@ -2568,22 +2811,25 @@
         <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F12" t="s">
-        <v>68</v>
+        <v>118</v>
+      </c>
+      <c r="G12" t="s">
+        <v>120</v>
       </c>
       <c r="H12" t="s">
         <v>21</v>
       </c>
       <c r="I12" t="s">
-        <v>66</v>
+        <v>117</v>
       </c>
       <c r="J12" t="n">
-        <v>0.0</v>
+        <v>14.0</v>
       </c>
     </row>
   </sheetData>
@@ -2607,12 +2853,12 @@
     <col min="1" max="1" width="17.02734375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="14.16796875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="19.84765625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="11.08984375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="9.9765625" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="9.9765625" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="21.2734375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="13.28515625" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="14.6796875" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="11.7265625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="13.06640625" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="13.19140625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="30.0" customHeight="true">
@@ -2625,7 +2871,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s" s="178">
-        <v>69</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4">
@@ -2633,7 +2879,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s" s="180">
-        <v>70</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5">
@@ -2685,16 +2931,19 @@
         <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>71</v>
+        <v>126</v>
+      </c>
+      <c r="G6" t="s">
+        <v>127</v>
       </c>
       <c r="H6" t="s">
         <v>21</v>
       </c>
       <c r="I6" t="s">
-        <v>69</v>
+        <v>125</v>
       </c>
       <c r="J6" t="n">
-        <v>7.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="7">
@@ -2714,21 +2963,24 @@
         <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>71</v>
+        <v>126</v>
+      </c>
+      <c r="G7" t="s">
+        <v>128</v>
       </c>
       <c r="H7" t="s">
         <v>21</v>
       </c>
       <c r="I7" t="s">
-        <v>69</v>
+        <v>125</v>
       </c>
       <c r="J7" t="n">
-        <v>12.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
@@ -2737,27 +2989,30 @@
         <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F8" t="s">
-        <v>71</v>
+        <v>126</v>
+      </c>
+      <c r="G8" t="s">
+        <v>129</v>
       </c>
       <c r="H8" t="s">
         <v>21</v>
       </c>
       <c r="I8" t="s">
-        <v>69</v>
+        <v>125</v>
       </c>
       <c r="J8" t="n">
-        <v>12.0</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
         <v>16</v>
@@ -2766,27 +3021,30 @@
         <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F9" t="s">
-        <v>71</v>
+        <v>126</v>
+      </c>
+      <c r="G9" t="s">
+        <v>130</v>
       </c>
       <c r="H9" t="s">
         <v>21</v>
       </c>
       <c r="I9" t="s">
-        <v>69</v>
+        <v>125</v>
       </c>
       <c r="J9" t="n">
-        <v>5.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
         <v>16</v>
@@ -2795,27 +3053,30 @@
         <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F10" t="s">
-        <v>71</v>
+        <v>126</v>
+      </c>
+      <c r="G10" t="s">
+        <v>130</v>
       </c>
       <c r="H10" t="s">
         <v>21</v>
       </c>
       <c r="I10" t="s">
-        <v>69</v>
+        <v>125</v>
       </c>
       <c r="J10" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
         <v>16</v>
@@ -2824,27 +3085,30 @@
         <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="F11" t="s">
-        <v>71</v>
+        <v>126</v>
+      </c>
+      <c r="G11" t="s">
+        <v>131</v>
       </c>
       <c r="H11" t="s">
         <v>21</v>
       </c>
       <c r="I11" t="s">
-        <v>69</v>
+        <v>125</v>
       </c>
       <c r="J11" t="n">
-        <v>14.0</v>
+        <v>16.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B12" t="s">
         <v>16</v>
@@ -2853,19 +3117,22 @@
         <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F12" t="s">
-        <v>71</v>
+        <v>126</v>
+      </c>
+      <c r="G12" t="s">
+        <v>132</v>
       </c>
       <c r="H12" t="s">
         <v>21</v>
       </c>
       <c r="I12" t="s">
-        <v>69</v>
+        <v>125</v>
       </c>
       <c r="J12" t="n">
         <v>1.0</v>
@@ -2892,12 +3159,12 @@
     <col min="1" max="1" width="17.02734375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="14.16796875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="19.84765625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="11.08984375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="9.9765625" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="9.9765625" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="21.2734375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="13.28515625" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="14.6796875" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="11.7265625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="13.7421875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="13.2734375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="30.0" customHeight="true">
@@ -2910,7 +3177,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s" s="28">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4">
@@ -2918,7 +3185,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s" s="30">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5">
@@ -2970,16 +3237,19 @@
         <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>41</v>
+        <v>45</v>
+      </c>
+      <c r="G6" t="s">
+        <v>46</v>
       </c>
       <c r="H6" t="s">
         <v>21</v>
       </c>
       <c r="I6" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="J6" t="n">
-        <v>4.0</v>
+        <v>19.0</v>
       </c>
     </row>
     <row r="7">
@@ -2999,13 +3269,16 @@
         <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>41</v>
+        <v>45</v>
+      </c>
+      <c r="G7" t="s">
+        <v>47</v>
       </c>
       <c r="H7" t="s">
         <v>21</v>
       </c>
       <c r="I7" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="J7" t="n">
         <v>9.0</v>
@@ -3013,7 +3286,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
@@ -3022,27 +3295,30 @@
         <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F8" t="s">
-        <v>41</v>
+        <v>45</v>
+      </c>
+      <c r="G8" t="s">
+        <v>48</v>
       </c>
       <c r="H8" t="s">
         <v>21</v>
       </c>
       <c r="I8" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="J8" t="n">
-        <v>10.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
         <v>16</v>
@@ -3051,27 +3327,30 @@
         <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F9" t="s">
-        <v>41</v>
+        <v>45</v>
+      </c>
+      <c r="G9" t="s">
+        <v>49</v>
       </c>
       <c r="H9" t="s">
         <v>21</v>
       </c>
       <c r="I9" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="J9" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
         <v>16</v>
@@ -3080,19 +3359,22 @@
         <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F10" t="s">
-        <v>41</v>
+        <v>45</v>
+      </c>
+      <c r="G10" t="s">
+        <v>45</v>
       </c>
       <c r="H10" t="s">
         <v>21</v>
       </c>
       <c r="I10" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="J10" t="n">
         <v>10.0</v>
@@ -3100,7 +3382,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
         <v>16</v>
@@ -3109,27 +3391,30 @@
         <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="F11" t="s">
-        <v>41</v>
+        <v>45</v>
+      </c>
+      <c r="G11" t="s">
+        <v>49</v>
       </c>
       <c r="H11" t="s">
         <v>21</v>
       </c>
       <c r="I11" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="J11" t="n">
-        <v>14.0</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B12" t="s">
         <v>16</v>
@@ -3138,22 +3423,25 @@
         <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F12" t="s">
-        <v>41</v>
+        <v>45</v>
+      </c>
+      <c r="G12" t="s">
+        <v>50</v>
       </c>
       <c r="H12" t="s">
         <v>21</v>
       </c>
       <c r="I12" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="J12" t="n">
-        <v>6.0</v>
+        <v>14.0</v>
       </c>
     </row>
   </sheetData>
@@ -3177,12 +3465,12 @@
     <col min="1" max="1" width="17.02734375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="14.16796875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="19.84765625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="11.08984375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="9.9765625" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="9.9765625" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="21.2734375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="13.28515625" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="14.6796875" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="11.7265625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="12.91796875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="13.87890625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="30.0" customHeight="true">
@@ -3195,7 +3483,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s" s="43">
-        <v>42</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4">
@@ -3203,7 +3491,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s" s="45">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5">
@@ -3255,16 +3543,19 @@
         <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>44</v>
+        <v>48</v>
+      </c>
+      <c r="G6" t="s">
+        <v>52</v>
       </c>
       <c r="H6" t="s">
         <v>21</v>
       </c>
       <c r="I6" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="J6" t="n">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="7">
@@ -3284,21 +3575,24 @@
         <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>44</v>
+        <v>48</v>
+      </c>
+      <c r="G7" t="s">
+        <v>53</v>
       </c>
       <c r="H7" t="s">
         <v>21</v>
       </c>
       <c r="I7" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="J7" t="n">
-        <v>4.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
@@ -3307,27 +3601,30 @@
         <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F8" t="s">
-        <v>44</v>
+        <v>48</v>
+      </c>
+      <c r="G8" t="s">
+        <v>54</v>
       </c>
       <c r="H8" t="s">
         <v>21</v>
       </c>
       <c r="I8" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="J8" t="n">
-        <v>1.0</v>
+        <v>16.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
         <v>16</v>
@@ -3336,27 +3633,30 @@
         <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F9" t="s">
-        <v>44</v>
+        <v>48</v>
+      </c>
+      <c r="G9" t="s">
+        <v>55</v>
       </c>
       <c r="H9" t="s">
         <v>21</v>
       </c>
       <c r="I9" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="J9" t="n">
-        <v>14.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
         <v>16</v>
@@ -3365,27 +3665,30 @@
         <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F10" t="s">
-        <v>44</v>
+        <v>48</v>
+      </c>
+      <c r="G10" t="s">
+        <v>56</v>
       </c>
       <c r="H10" t="s">
         <v>21</v>
       </c>
       <c r="I10" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="J10" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
         <v>16</v>
@@ -3394,27 +3697,30 @@
         <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="F11" t="s">
-        <v>44</v>
+        <v>48</v>
+      </c>
+      <c r="G11" t="s">
+        <v>57</v>
       </c>
       <c r="H11" t="s">
         <v>21</v>
       </c>
       <c r="I11" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="J11" t="n">
-        <v>19.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B12" t="s">
         <v>16</v>
@@ -3423,22 +3729,25 @@
         <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F12" t="s">
-        <v>44</v>
+        <v>48</v>
+      </c>
+      <c r="G12" t="s">
+        <v>58</v>
       </c>
       <c r="H12" t="s">
         <v>21</v>
       </c>
       <c r="I12" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="J12" t="n">
-        <v>1.0</v>
+        <v>9.0</v>
       </c>
     </row>
   </sheetData>
@@ -3462,12 +3771,12 @@
     <col min="1" max="1" width="17.02734375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="14.16796875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="19.84765625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="11.08984375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="9.9765625" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="9.9765625" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="21.2734375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="13.28515625" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="14.6796875" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="11.7265625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="12.9921875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="13.00390625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="30.0" customHeight="true">
@@ -3480,7 +3789,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s" s="58">
-        <v>45</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4">
@@ -3488,7 +3797,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s" s="60">
-        <v>46</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5">
@@ -3540,16 +3849,19 @@
         <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>47</v>
+        <v>60</v>
+      </c>
+      <c r="G6" t="s">
+        <v>61</v>
       </c>
       <c r="H6" t="s">
         <v>21</v>
       </c>
       <c r="I6" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="J6" t="n">
-        <v>12.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="7">
@@ -3569,21 +3881,24 @@
         <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>47</v>
+        <v>60</v>
+      </c>
+      <c r="G7" t="s">
+        <v>62</v>
       </c>
       <c r="H7" t="s">
         <v>21</v>
       </c>
       <c r="I7" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="J7" t="n">
-        <v>18.0</v>
+        <v>14.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
@@ -3592,27 +3907,30 @@
         <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F8" t="s">
-        <v>47</v>
+        <v>60</v>
+      </c>
+      <c r="G8" t="s">
+        <v>63</v>
       </c>
       <c r="H8" t="s">
         <v>21</v>
       </c>
       <c r="I8" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="J8" t="n">
-        <v>7.0</v>
+        <v>14.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
         <v>16</v>
@@ -3621,27 +3939,30 @@
         <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F9" t="s">
-        <v>47</v>
+        <v>60</v>
+      </c>
+      <c r="G9" t="s">
+        <v>64</v>
       </c>
       <c r="H9" t="s">
         <v>21</v>
       </c>
       <c r="I9" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="J9" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
         <v>16</v>
@@ -3650,27 +3971,30 @@
         <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F10" t="s">
-        <v>47</v>
+        <v>60</v>
+      </c>
+      <c r="G10" t="s">
+        <v>65</v>
       </c>
       <c r="H10" t="s">
         <v>21</v>
       </c>
       <c r="I10" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="J10" t="n">
-        <v>2.0</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
         <v>16</v>
@@ -3679,27 +4003,30 @@
         <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="F11" t="s">
-        <v>47</v>
+        <v>60</v>
+      </c>
+      <c r="G11" t="s">
+        <v>66</v>
       </c>
       <c r="H11" t="s">
         <v>21</v>
       </c>
       <c r="I11" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="J11" t="n">
-        <v>13.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B12" t="s">
         <v>16</v>
@@ -3708,22 +4035,25 @@
         <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F12" t="s">
-        <v>47</v>
+        <v>60</v>
+      </c>
+      <c r="G12" t="s">
+        <v>67</v>
       </c>
       <c r="H12" t="s">
         <v>21</v>
       </c>
       <c r="I12" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="J12" t="n">
-        <v>18.0</v>
+        <v>12.0</v>
       </c>
     </row>
   </sheetData>
@@ -3747,12 +4077,12 @@
     <col min="1" max="1" width="17.02734375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="14.16796875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="19.84765625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="11.08984375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="9.9765625" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="9.9765625" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="21.2734375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="13.28515625" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="14.6796875" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="11.7265625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="12.98828125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="13.5625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="30.0" customHeight="true">
@@ -3765,7 +4095,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s" s="73">
-        <v>48</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4">
@@ -3773,7 +4103,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s" s="75">
-        <v>49</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5">
@@ -3825,16 +4155,19 @@
         <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>50</v>
+        <v>69</v>
+      </c>
+      <c r="G6" t="s">
+        <v>70</v>
       </c>
       <c r="H6" t="s">
         <v>21</v>
       </c>
       <c r="I6" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="J6" t="n">
-        <v>15.0</v>
+        <v>18.0</v>
       </c>
     </row>
     <row r="7">
@@ -3854,21 +4187,24 @@
         <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>50</v>
+        <v>69</v>
+      </c>
+      <c r="G7" t="s">
+        <v>71</v>
       </c>
       <c r="H7" t="s">
         <v>21</v>
       </c>
       <c r="I7" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="J7" t="n">
-        <v>17.0</v>
+        <v>19.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
@@ -3877,27 +4213,30 @@
         <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F8" t="s">
-        <v>50</v>
+        <v>69</v>
+      </c>
+      <c r="G8" t="s">
+        <v>72</v>
       </c>
       <c r="H8" t="s">
         <v>21</v>
       </c>
       <c r="I8" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="J8" t="n">
-        <v>5.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
         <v>16</v>
@@ -3906,27 +4245,30 @@
         <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F9" t="s">
-        <v>50</v>
+        <v>69</v>
+      </c>
+      <c r="G9" t="s">
+        <v>73</v>
       </c>
       <c r="H9" t="s">
         <v>21</v>
       </c>
       <c r="I9" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="J9" t="n">
-        <v>9.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
         <v>16</v>
@@ -3935,27 +4277,30 @@
         <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F10" t="s">
-        <v>50</v>
+        <v>69</v>
+      </c>
+      <c r="G10" t="s">
+        <v>74</v>
       </c>
       <c r="H10" t="s">
         <v>21</v>
       </c>
       <c r="I10" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="J10" t="n">
-        <v>10.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
         <v>16</v>
@@ -3964,27 +4309,30 @@
         <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="F11" t="s">
-        <v>50</v>
+        <v>69</v>
+      </c>
+      <c r="G11" t="s">
+        <v>75</v>
       </c>
       <c r="H11" t="s">
         <v>21</v>
       </c>
       <c r="I11" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="J11" t="n">
-        <v>10.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B12" t="s">
         <v>16</v>
@@ -3993,22 +4341,25 @@
         <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F12" t="s">
-        <v>50</v>
+        <v>69</v>
+      </c>
+      <c r="G12" t="s">
+        <v>76</v>
       </c>
       <c r="H12" t="s">
         <v>21</v>
       </c>
       <c r="I12" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="J12" t="n">
-        <v>14.0</v>
+        <v>15.0</v>
       </c>
     </row>
   </sheetData>
@@ -4032,9 +4383,9 @@
     <col min="1" max="1" width="17.02734375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="14.16796875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="19.84765625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="11.08984375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="9.9765625" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="9.9765625" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="21.2734375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="13.28515625" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="14.6796875" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="11.7265625" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="12.91796875" customWidth="true" bestFit="true"/>
@@ -4050,7 +4401,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s" s="88">
-        <v>51</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4">
@@ -4058,7 +4409,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s" s="90">
-        <v>52</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5">
@@ -4110,16 +4461,19 @@
         <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>53</v>
+        <v>78</v>
+      </c>
+      <c r="G6" t="s">
+        <v>79</v>
       </c>
       <c r="H6" t="s">
         <v>21</v>
       </c>
       <c r="I6" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="J6" t="n">
-        <v>19.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="7">
@@ -4139,21 +4493,24 @@
         <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>53</v>
+        <v>78</v>
+      </c>
+      <c r="G7" t="s">
+        <v>80</v>
       </c>
       <c r="H7" t="s">
         <v>21</v>
       </c>
       <c r="I7" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="J7" t="n">
-        <v>9.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
@@ -4162,27 +4519,30 @@
         <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F8" t="s">
-        <v>53</v>
+        <v>78</v>
+      </c>
+      <c r="G8" t="s">
+        <v>81</v>
       </c>
       <c r="H8" t="s">
         <v>21</v>
       </c>
       <c r="I8" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="J8" t="n">
-        <v>13.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
         <v>16</v>
@@ -4191,27 +4551,30 @@
         <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F9" t="s">
-        <v>53</v>
+        <v>78</v>
+      </c>
+      <c r="G9" t="s">
+        <v>82</v>
       </c>
       <c r="H9" t="s">
         <v>21</v>
       </c>
       <c r="I9" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="J9" t="n">
-        <v>16.0</v>
+        <v>18.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
         <v>16</v>
@@ -4220,27 +4583,30 @@
         <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F10" t="s">
-        <v>53</v>
+        <v>78</v>
+      </c>
+      <c r="G10" t="s">
+        <v>83</v>
       </c>
       <c r="H10" t="s">
         <v>21</v>
       </c>
       <c r="I10" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="J10" t="n">
-        <v>3.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
         <v>16</v>
@@ -4249,27 +4615,30 @@
         <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="F11" t="s">
-        <v>53</v>
+        <v>78</v>
+      </c>
+      <c r="G11" t="s">
+        <v>84</v>
       </c>
       <c r="H11" t="s">
         <v>21</v>
       </c>
       <c r="I11" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="J11" t="n">
-        <v>15.0</v>
+        <v>17.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B12" t="s">
         <v>16</v>
@@ -4278,22 +4647,25 @@
         <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F12" t="s">
-        <v>53</v>
+        <v>78</v>
+      </c>
+      <c r="G12" t="s">
+        <v>85</v>
       </c>
       <c r="H12" t="s">
         <v>21</v>
       </c>
       <c r="I12" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="J12" t="n">
-        <v>17.0</v>
+        <v>4.0</v>
       </c>
     </row>
   </sheetData>
@@ -4317,12 +4689,12 @@
     <col min="1" max="1" width="17.02734375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="14.16796875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="19.84765625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="11.08984375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="9.9765625" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="9.9765625" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="21.2734375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="13.28515625" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="14.6796875" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="11.7265625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="14.68359375" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="12.91796875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="30.0" customHeight="true">
@@ -4335,7 +4707,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s" s="103">
-        <v>54</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4">
@@ -4343,7 +4715,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s" s="105">
-        <v>55</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5">
@@ -4395,16 +4767,19 @@
         <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>56</v>
+        <v>87</v>
+      </c>
+      <c r="G6" t="s">
+        <v>88</v>
       </c>
       <c r="H6" t="s">
         <v>21</v>
       </c>
       <c r="I6" t="s">
-        <v>54</v>
+        <v>86</v>
       </c>
       <c r="J6" t="n">
-        <v>10.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="7">
@@ -4424,21 +4799,24 @@
         <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>56</v>
+        <v>87</v>
+      </c>
+      <c r="G7" t="s">
+        <v>89</v>
       </c>
       <c r="H7" t="s">
         <v>21</v>
       </c>
       <c r="I7" t="s">
-        <v>54</v>
+        <v>86</v>
       </c>
       <c r="J7" t="n">
-        <v>15.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
@@ -4447,27 +4825,30 @@
         <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F8" t="s">
-        <v>56</v>
+        <v>87</v>
+      </c>
+      <c r="G8" t="s">
+        <v>90</v>
       </c>
       <c r="H8" t="s">
         <v>21</v>
       </c>
       <c r="I8" t="s">
-        <v>54</v>
+        <v>86</v>
       </c>
       <c r="J8" t="n">
-        <v>10.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
         <v>16</v>
@@ -4476,27 +4857,30 @@
         <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F9" t="s">
-        <v>56</v>
+        <v>87</v>
+      </c>
+      <c r="G9" t="s">
+        <v>91</v>
       </c>
       <c r="H9" t="s">
         <v>21</v>
       </c>
       <c r="I9" t="s">
-        <v>54</v>
+        <v>86</v>
       </c>
       <c r="J9" t="n">
-        <v>10.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
         <v>16</v>
@@ -4505,27 +4889,30 @@
         <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F10" t="s">
-        <v>56</v>
+        <v>87</v>
+      </c>
+      <c r="G10" t="s">
+        <v>92</v>
       </c>
       <c r="H10" t="s">
         <v>21</v>
       </c>
       <c r="I10" t="s">
-        <v>54</v>
+        <v>86</v>
       </c>
       <c r="J10" t="n">
-        <v>9.0</v>
+        <v>14.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
         <v>16</v>
@@ -4534,19 +4921,22 @@
         <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="F11" t="s">
-        <v>56</v>
+        <v>87</v>
+      </c>
+      <c r="G11" t="s">
+        <v>91</v>
       </c>
       <c r="H11" t="s">
         <v>21</v>
       </c>
       <c r="I11" t="s">
-        <v>54</v>
+        <v>86</v>
       </c>
       <c r="J11" t="n">
         <v>2.0</v>
@@ -4554,7 +4944,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B12" t="s">
         <v>16</v>
@@ -4563,22 +4953,25 @@
         <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F12" t="s">
-        <v>56</v>
+        <v>87</v>
+      </c>
+      <c r="G12" t="s">
+        <v>93</v>
       </c>
       <c r="H12" t="s">
         <v>21</v>
       </c>
       <c r="I12" t="s">
-        <v>54</v>
+        <v>86</v>
       </c>
       <c r="J12" t="n">
-        <v>15.0</v>
+        <v>8.0</v>
       </c>
     </row>
   </sheetData>
@@ -4602,9 +4995,9 @@
     <col min="1" max="1" width="17.02734375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="14.16796875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="19.84765625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="11.08984375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="9.9765625" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="9.9765625" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="21.2734375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="13.28515625" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="14.6796875" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="11.7265625" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="12.91796875" customWidth="true" bestFit="true"/>
@@ -4620,7 +5013,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s" s="118">
-        <v>57</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4">
@@ -4628,7 +5021,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s" s="120">
-        <v>58</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5">
@@ -4680,16 +5073,19 @@
         <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>59</v>
+        <v>95</v>
+      </c>
+      <c r="G6" t="s">
+        <v>96</v>
       </c>
       <c r="H6" t="s">
         <v>21</v>
       </c>
       <c r="I6" t="s">
-        <v>57</v>
+        <v>94</v>
       </c>
       <c r="J6" t="n">
-        <v>18.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="7">
@@ -4709,21 +5105,24 @@
         <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>59</v>
+        <v>95</v>
+      </c>
+      <c r="G7" t="s">
+        <v>97</v>
       </c>
       <c r="H7" t="s">
         <v>21</v>
       </c>
       <c r="I7" t="s">
-        <v>57</v>
+        <v>94</v>
       </c>
       <c r="J7" t="n">
-        <v>0.0</v>
+        <v>11.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
@@ -4732,27 +5131,30 @@
         <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F8" t="s">
-        <v>59</v>
+        <v>95</v>
+      </c>
+      <c r="G8" t="s">
+        <v>98</v>
       </c>
       <c r="H8" t="s">
         <v>21</v>
       </c>
       <c r="I8" t="s">
-        <v>57</v>
+        <v>94</v>
       </c>
       <c r="J8" t="n">
-        <v>10.0</v>
+        <v>18.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
         <v>16</v>
@@ -4761,19 +5163,22 @@
         <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F9" t="s">
-        <v>59</v>
+        <v>95</v>
+      </c>
+      <c r="G9" t="s">
+        <v>99</v>
       </c>
       <c r="H9" t="s">
         <v>21</v>
       </c>
       <c r="I9" t="s">
-        <v>57</v>
+        <v>94</v>
       </c>
       <c r="J9" t="n">
         <v>16.0</v>
@@ -4781,7 +5186,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
         <v>16</v>
@@ -4790,27 +5195,30 @@
         <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F10" t="s">
-        <v>59</v>
+        <v>95</v>
+      </c>
+      <c r="G10" t="s">
+        <v>100</v>
       </c>
       <c r="H10" t="s">
         <v>21</v>
       </c>
       <c r="I10" t="s">
-        <v>57</v>
+        <v>94</v>
       </c>
       <c r="J10" t="n">
-        <v>4.0</v>
+        <v>17.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
         <v>16</v>
@@ -4819,27 +5227,30 @@
         <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="F11" t="s">
-        <v>59</v>
+        <v>95</v>
+      </c>
+      <c r="G11" t="s">
+        <v>101</v>
       </c>
       <c r="H11" t="s">
         <v>21</v>
       </c>
       <c r="I11" t="s">
-        <v>57</v>
+        <v>94</v>
       </c>
       <c r="J11" t="n">
-        <v>9.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B12" t="s">
         <v>16</v>
@@ -4848,22 +5259,25 @@
         <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F12" t="s">
-        <v>59</v>
+        <v>95</v>
+      </c>
+      <c r="G12" t="s">
+        <v>102</v>
       </c>
       <c r="H12" t="s">
         <v>21</v>
       </c>
       <c r="I12" t="s">
-        <v>57</v>
+        <v>94</v>
       </c>
       <c r="J12" t="n">
-        <v>6.0</v>
+        <v>3.0</v>
       </c>
     </row>
   </sheetData>
@@ -4887,12 +5301,12 @@
     <col min="1" max="1" width="17.02734375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="14.16796875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="19.84765625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="11.08984375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="9.9765625" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="9.9765625" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="21.2734375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="13.28515625" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="14.6796875" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="11.7265625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="12.984375" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="14.19140625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="30.0" customHeight="true">
@@ -4905,7 +5319,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s" s="133">
-        <v>60</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4">
@@ -4913,7 +5327,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s" s="135">
-        <v>61</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5">
@@ -4965,16 +5379,19 @@
         <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>62</v>
+        <v>104</v>
+      </c>
+      <c r="G6" t="s">
+        <v>105</v>
       </c>
       <c r="H6" t="s">
         <v>21</v>
       </c>
       <c r="I6" t="s">
-        <v>60</v>
+        <v>103</v>
       </c>
       <c r="J6" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="7">
@@ -4994,21 +5411,24 @@
         <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>62</v>
+        <v>104</v>
+      </c>
+      <c r="G7" t="s">
+        <v>106</v>
       </c>
       <c r="H7" t="s">
         <v>21</v>
       </c>
       <c r="I7" t="s">
-        <v>60</v>
+        <v>103</v>
       </c>
       <c r="J7" t="n">
-        <v>18.0</v>
+        <v>11.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
@@ -5017,27 +5437,30 @@
         <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F8" t="s">
-        <v>62</v>
+        <v>104</v>
+      </c>
+      <c r="G8" t="s">
+        <v>107</v>
       </c>
       <c r="H8" t="s">
         <v>21</v>
       </c>
       <c r="I8" t="s">
-        <v>60</v>
+        <v>103</v>
       </c>
       <c r="J8" t="n">
-        <v>7.0</v>
+        <v>19.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
         <v>16</v>
@@ -5046,27 +5469,30 @@
         <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F9" t="s">
-        <v>62</v>
+        <v>104</v>
+      </c>
+      <c r="G9" t="s">
+        <v>108</v>
       </c>
       <c r="H9" t="s">
         <v>21</v>
       </c>
       <c r="I9" t="s">
-        <v>60</v>
+        <v>103</v>
       </c>
       <c r="J9" t="n">
-        <v>11.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
         <v>16</v>
@@ -5075,27 +5501,30 @@
         <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F10" t="s">
-        <v>62</v>
+        <v>104</v>
+      </c>
+      <c r="G10" t="s">
+        <v>109</v>
       </c>
       <c r="H10" t="s">
         <v>21</v>
       </c>
       <c r="I10" t="s">
-        <v>60</v>
+        <v>103</v>
       </c>
       <c r="J10" t="n">
-        <v>10.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
         <v>16</v>
@@ -5104,27 +5533,30 @@
         <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="F11" t="s">
-        <v>62</v>
+        <v>104</v>
+      </c>
+      <c r="G11" t="s">
+        <v>108</v>
       </c>
       <c r="H11" t="s">
         <v>21</v>
       </c>
       <c r="I11" t="s">
-        <v>60</v>
+        <v>103</v>
       </c>
       <c r="J11" t="n">
-        <v>10.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B12" t="s">
         <v>16</v>
@@ -5133,22 +5565,25 @@
         <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F12" t="s">
-        <v>62</v>
+        <v>104</v>
+      </c>
+      <c r="G12" t="s">
+        <v>109</v>
       </c>
       <c r="H12" t="s">
         <v>21</v>
       </c>
       <c r="I12" t="s">
-        <v>60</v>
+        <v>103</v>
       </c>
       <c r="J12" t="n">
-        <v>9.0</v>
+        <v>18.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>